<commit_message>
Atualizacao do UC 7 (Output)
</commit_message>
<xml_diff>
--- a/output/xlsx/UC007 - Enviar Mensagem de Contato--GT-.xlsx
+++ b/output/xlsx/UC007 - Enviar Mensagem de Contato--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="57">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -110,79 +110,79 @@
     <t>SYSTEM apresenta o e-mail informado</t>
   </si>
   <si>
+    <t>Usuário do Sistema seleciona 'Sugestão' como tipo de mensagem</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta o tipo de mensagem selecionado</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona faixa etária 'Entre 30 e 60 anos'</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta a faixa de idade selecionada</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema escreve o conteúdo da mensagem</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta o conteúdo da mensagem informado</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema submete o formulário</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem de erro solicitando preenchimento do conteúdo</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem de erro solicitando escolha pelo tipo de mensagem</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona 'Reclamação' como tipo de mensagem</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema mantida faixa etária selecionada por padrão: 'Menor que 18 anos'</t>
+  </si>
+  <si>
+    <t>SYSTEM processa e envia a mensagem</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza mensagem de confirmação</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'Mensagem de &lt;tipo de mensagem&gt; por usuário de idade &lt;faixa de idade&gt; foi enviada com sucesso'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Mensagem de contato foi enviada com sucesso para a administração</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona o tipo de mensagem</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona faixa etária 'Acima de 60 anos'</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem de erro solicitando e-mail válido</t>
+  </si>
+  <si>
     <t>Usuário do Sistema seleciona 'Dúvida' como tipo de mensagem</t>
   </si>
   <si>
-    <t>SYSTEM apresenta o tipo de mensagem selecionado</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona faixa etária 'Entre 30 e 60 anos'</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta a faixa de idade selecionada</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema escreve o conteúdo da mensagem</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta o conteúdo da mensagem informado</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema submete o formulário</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem de erro solicitando e-mail válido</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona 'Reclamação' como tipo de mensagem</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona faixa etária 'Menor que 18 anos'</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Sua mensagem não pôde ser enviada no momento! Tente mais tarde.' (MSG004)</t>
-  </si>
-  <si>
-    <t>SYSTEM processa e envia a mensagem</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza mensagem de confirmação</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Mensagem de &lt;tipo de mensagem&gt; por usuário de idade &lt;faixa de idade&gt; foi enviada com sucesso'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Mensagem de contato foi enviada com sucesso para a administração</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona 'Sugestão' como tipo de mensagem</t>
-  </si>
-  <si>
     <t>Usuário do Sistema seleciona faixa etária 'Entre 18 e 29 anos'</t>
   </si>
   <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona a faixa de idade</t>
+  </si>
+  <si>
     <t>SYSTEM exibe mensagem de erro solicitando preenchimento do nome</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona o tipo de mensagem</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona a faixa de idade</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona faixa etária 'Acima de 60 anos'</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem de erro solicitando preenchimento do conteúdo</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -679,13 +679,13 @@
         <v>8.0</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D17" t="s" s="7">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s" s="6">
         <v>2</v>
@@ -699,13 +699,13 @@
         <v>9.0</v>
       </c>
       <c r="B18" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s" s="7">
         <v>40</v>
-      </c>
-      <c r="C18" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s" s="7">
-        <v>33</v>
       </c>
       <c r="E18" t="s" s="6">
         <v>2</v>
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s" s="6">
         <v>2</v>
@@ -739,13 +739,13 @@
         <v>11.0</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D20" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s" s="6">
         <v>2</v>
@@ -759,13 +759,13 @@
         <v>12.0</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D21" t="s" s="7">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s" s="6">
         <v>2</v>
@@ -1061,13 +1061,13 @@
         <v>8.0</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D38" t="s" s="7">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E38" t="s" s="6">
         <v>2</v>
@@ -1081,13 +1081,13 @@
         <v>9.0</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D39" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s" s="6">
         <v>2</v>
@@ -1101,13 +1101,13 @@
         <v>10.0</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E40" t="s" s="6">
         <v>2</v>
@@ -1121,13 +1121,13 @@
         <v>11.0</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D41" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E41" t="s" s="6">
         <v>2</v>
@@ -1141,13 +1141,13 @@
         <v>12.0</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D42" t="s" s="7">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s" s="6">
         <v>2</v>
@@ -1161,13 +1161,13 @@
         <v>13.0</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D43" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E43" t="s" s="6">
         <v>2</v>
@@ -1177,139 +1177,139 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n" s="10">
-        <v>14.0</v>
-      </c>
-      <c r="B44" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E44" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F44" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="8">
+      <c r="A44" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="B45" t="s" s="8">
+      <c r="B44" t="s" s="8">
         <v>47</v>
       </c>
-      <c r="C45" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F45" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
+      <c r="C44" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45"/>
     <row r="46"/>
-    <row r="47"/>
+    <row r="47">
+      <c r="A47" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s" s="4">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="48">
-      <c r="A48" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s" s="4">
-        <v>54</v>
-      </c>
-      <c r="C48" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D48" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F48" t="s" s="4">
+      <c r="A48" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F49" t="s" s="9">
+      <c r="A49" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B50" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F50" t="s" s="8">
-        <v>2</v>
+      <c r="A50" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C50" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F50" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C51" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D51" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E51" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F51" t="s" s="5">
-        <v>25</v>
+      <c r="A51" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B51" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B52" t="s" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E52" t="s" s="6">
         <v>2</v>
@@ -1320,16 +1320,16 @@
     </row>
     <row r="53">
       <c r="A53" t="n" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B53" t="s" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s" s="6">
         <v>2</v>
@@ -1340,16 +1340,16 @@
     </row>
     <row r="54">
       <c r="A54" t="n" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s" s="6">
         <v>2</v>
@@ -1360,16 +1360,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E55" t="s" s="6">
         <v>2</v>
@@ -1380,16 +1380,16 @@
     </row>
     <row r="56">
       <c r="A56" t="n" s="10">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B56" t="s" s="7">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D56" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E56" t="s" s="6">
         <v>2</v>
@@ -1400,16 +1400,16 @@
     </row>
     <row r="57">
       <c r="A57" t="n" s="10">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B57" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C57" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D57" t="s" s="7">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s" s="6">
         <v>2</v>
@@ -1420,16 +1420,16 @@
     </row>
     <row r="58">
       <c r="A58" t="n" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B58" t="s" s="7">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D58" t="s" s="7">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="E58" t="s" s="6">
         <v>2</v>
@@ -1440,16 +1440,16 @@
     </row>
     <row r="59">
       <c r="A59" t="n" s="10">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B59" t="s" s="7">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E59" t="s" s="6">
         <v>2</v>
@@ -1460,16 +1460,16 @@
     </row>
     <row r="60">
       <c r="A60" t="n" s="10">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B60" t="s" s="7">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C60" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s" s="6">
         <v>2</v>
@@ -1480,41 +1480,101 @@
     </row>
     <row r="61">
       <c r="A61" t="n" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B61" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B62" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C62" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E62" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B63" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E63" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n" s="10">
+        <v>14.0</v>
+      </c>
+      <c r="B64" t="s" s="7">
         <v>44</v>
       </c>
-      <c r="C61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s" s="7">
+      <c r="C64" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="E61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="8">
+      <c r="E64" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="B62" t="s" s="8">
+      <c r="B65" t="s" s="8">
         <v>47</v>
       </c>
-      <c r="C62" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F62" t="s" s="8">
+      <c r="C65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1526,10 +1586,10 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B65:F65"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>